<commit_message>
removed authorization to view forum. typo fix registerHarvest.ejs
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>ac tree</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
   <si>
     <t>Tree</t>
@@ -489,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="7" width="10" customWidth="1"/>
@@ -542,10 +548,10 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>39.399</v>
+        <v>39.4921</v>
       </c>
       <c r="G2">
-        <v>-74.5146</v>
+        <v>-74.5323</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -656,6 +662,32 @@
       </c>
       <c r="H6" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44295</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>39.399</v>
+      </c>
+      <c r="G7">
+        <v>-74.5146</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -666,7 +698,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="4" width="10" customWidth="1"/>
@@ -674,16 +706,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -922,6 +954,34 @@
       </c>
       <c r="D18">
         <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44295</v>
+      </c>
+      <c r="D19">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44295</v>
+      </c>
+      <c r="D20">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -932,7 +992,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="10" customWidth="1"/>
@@ -943,25 +1003,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -984,7 +1044,7 @@
         <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1007,7 +1067,7 @@
         <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1030,7 +1090,30 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44295</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated database excel download
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -13,17 +13,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
-  <si>
-    <t>Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Tree ID</t>
   </si>
   <si>
     <t>Circumf</t>
   </si>
   <si>
-    <t>Stem Count</t>
-  </si>
-  <si>
     <t>Tapping Date</t>
   </si>
   <si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>End of Season Notes</t>
+  </si>
+  <si>
+    <t>tang</t>
   </si>
   <si>
     <t>Dingle</t>
@@ -535,11 +538,11 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
         <v>100</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>44286</v>
@@ -554,21 +557,21 @@
         <v>-74.5323</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
         <v>598</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
       </c>
       <c r="D3" s="1">
         <v>44288</v>
@@ -583,18 +586,18 @@
         <v>-74.5145</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
         <v>199</v>
-      </c>
-      <c r="C4">
-        <v>54</v>
       </c>
       <c r="D4" s="1">
         <v>44288</v>
@@ -609,18 +612,18 @@
         <v>-74.5323</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
         <v>100</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
       </c>
       <c r="D5" s="1">
         <v>44292</v>
@@ -635,18 +638,18 @@
         <v>-74.5146</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
         <v>121</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>44288</v>
@@ -661,18 +664,18 @@
         <v>-74.4444</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
         <v>44295</v>
@@ -687,7 +690,7 @@
         <v>-74.5146</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -706,21 +709,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -734,7 +737,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -748,7 +751,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>42</v>
@@ -762,7 +765,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>43</v>
@@ -776,7 +779,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>5365</v>
@@ -790,7 +793,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>353</v>
@@ -804,7 +807,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -818,7 +821,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>55</v>
@@ -832,7 +835,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>55</v>
@@ -846,7 +849,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>45</v>
@@ -860,7 +863,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>898</v>
@@ -874,7 +877,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>68</v>
@@ -888,7 +891,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>686</v>
@@ -902,7 +905,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>66</v>
@@ -916,7 +919,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>11</v>
@@ -930,7 +933,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>50</v>
@@ -944,7 +947,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>10</v>
@@ -958,7 +961,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>55</v>
@@ -972,7 +975,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -1003,25 +1006,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1044,7 +1047,7 @@
         <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1067,7 +1070,7 @@
         <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1090,7 +1093,7 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1113,7 +1116,7 @@
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added seasons data to excel database download and modified tree sheet to display most current season data
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Trees" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Saps" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Syrups" state="visible" r:id="rId6"/>
+    <sheet sheetId="2" name="Seasons" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Saps" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="Syrups" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="40">
   <si>
     <t>User</t>
   </si>
@@ -24,10 +25,16 @@
     <t>Circumf</t>
   </si>
   <si>
+    <t>Tap Height</t>
+  </si>
+  <si>
     <t>Tapping Date</t>
   </si>
   <si>
-    <t>Tap Height</t>
+    <t>First Season Flow</t>
+  </si>
+  <si>
+    <t>Last Season Flow</t>
   </si>
   <si>
     <t>Latitude</t>
@@ -45,40 +52,46 @@
     <t>tang</t>
   </si>
   <si>
-    <t>Dingle</t>
-  </si>
-  <si>
-    <t>I love this dingleTree</t>
-  </si>
-  <si>
-    <t>end of season 2</t>
-  </si>
-  <si>
-    <t>Oakey</t>
-  </si>
-  <si>
-    <t>Special oak tree that makes sap</t>
-  </si>
-  <si>
-    <t>stockton tree</t>
-  </si>
-  <si>
-    <t>software tree</t>
-  </si>
-  <si>
-    <t>ljk;jad</t>
-  </si>
-  <si>
-    <t>AC tree</t>
-  </si>
-  <si>
-    <t>ac tree</t>
+    <t>dasfasdfa</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>newaldfjads</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>example</t>
   </si>
   <si>
-    <t>notes</t>
+    <t>first season noteess</t>
+  </si>
+  <si>
+    <t>tree34</t>
+  </si>
+  <si>
+    <t>start of 2023</t>
+  </si>
+  <si>
+    <t>very long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notes</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>starting a new tree</t>
+  </si>
+  <si>
+    <t>end of season 2021</t>
+  </si>
+  <si>
+    <t>start of 2022</t>
   </si>
   <si>
     <t>Tree</t>
@@ -498,14 +511,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="7" width="10" customWidth="1"/>
-    <col min="8" max="9" width="30" customWidth="1"/>
+    <col min="1" max="5" width="10" customWidth="1"/>
+    <col min="6" max="7" width="15" customWidth="1"/>
+    <col min="8" max="9" width="10" customWidth="1"/>
+    <col min="10" max="11" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,163 +548,150 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44286</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>39.4921</v>
-      </c>
-      <c r="G2">
-        <v>-74.5323</v>
-      </c>
-      <c r="H2" t="s">
+        <v>5667</v>
+      </c>
+      <c r="D2">
+        <v>656</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44300</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>39.399</v>
+      </c>
+      <c r="I2">
+        <v>-74.5146</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>598</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44288</v>
-      </c>
-      <c r="E3">
+        <v>5667</v>
+      </c>
+      <c r="D3">
+        <v>656</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44300</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>39.399</v>
+      </c>
+      <c r="I3">
+        <v>-74.5146</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>44</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44299</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44301</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>39.3989</v>
+      </c>
+      <c r="I4">
+        <v>-74.5145</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45000</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44671</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44671</v>
+      </c>
+      <c r="H5">
+        <v>39.399</v>
+      </c>
+      <c r="I5">
+        <v>-74.5146</v>
+      </c>
+      <c r="J5" t="s">
         <v>20</v>
       </c>
-      <c r="F3">
-        <v>39.399</v>
-      </c>
-      <c r="G3">
-        <v>-74.5145</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>199</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44288</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>39.4921</v>
-      </c>
-      <c r="G4">
-        <v>-74.5323</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44292</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>39.3989</v>
-      </c>
-      <c r="G5">
-        <v>-74.5146</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>121</v>
-      </c>
-      <c r="D6" s="1">
-        <v>44288</v>
-      </c>
-      <c r="E6">
-        <v>121</v>
-      </c>
-      <c r="F6">
-        <v>39.3521</v>
-      </c>
-      <c r="G6">
-        <v>-74.4444</v>
-      </c>
-      <c r="H6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1">
-        <v>44295</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>39.399</v>
-      </c>
-      <c r="G7">
-        <v>-74.5146</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="K5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -701,7 +703,205 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:H7"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="4" width="10" customWidth="1"/>
+    <col min="5" max="6" width="15" customWidth="1"/>
+    <col min="7" max="8" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>2021</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44300</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44300</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>2021</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44299</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44301</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>2021</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44301</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>2022</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44664</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44671</v>
+      </c>
+      <c r="F6" s="1">
+        <v>44671</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>2023</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="4" width="10" customWidth="1"/>
@@ -709,282 +909,170 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
-        <v>44286</v>
+        <v>44300</v>
       </c>
       <c r="D2">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1">
-        <v>44271</v>
+        <v>44302</v>
       </c>
       <c r="D3">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>44268</v>
+        <v>44301</v>
       </c>
       <c r="D4">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>44286</v>
+        <v>44308</v>
       </c>
       <c r="D5">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>5365</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>44265</v>
+        <v>44302</v>
       </c>
       <c r="D6">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>353</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1">
-        <v>44281</v>
+        <v>44310</v>
       </c>
       <c r="D7">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>44277</v>
+        <v>44306</v>
       </c>
       <c r="D8">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1">
-        <v>44273</v>
+        <v>44291</v>
       </c>
       <c r="D9">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1">
-        <v>44266</v>
+        <v>44308</v>
       </c>
       <c r="D10">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B11">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1">
-        <v>44271</v>
+        <v>44314</v>
       </c>
       <c r="D11">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>898</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1">
-        <v>44282</v>
+        <v>44671</v>
       </c>
       <c r="D12">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>68</v>
-      </c>
-      <c r="C13" s="1">
-        <v>44289</v>
-      </c>
-      <c r="D13">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>686</v>
-      </c>
-      <c r="C14" s="1">
-        <v>44258</v>
-      </c>
-      <c r="D14">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>66</v>
-      </c>
-      <c r="C15" s="1">
-        <v>44270</v>
-      </c>
-      <c r="D15">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1">
-        <v>44287</v>
-      </c>
-      <c r="D16">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17">
-        <v>50</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44288</v>
-      </c>
-      <c r="D17">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18" s="1">
-        <v>44288</v>
-      </c>
-      <c r="D18">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19">
-        <v>55</v>
-      </c>
-      <c r="C19" s="1">
-        <v>44295</v>
-      </c>
-      <c r="D19">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>10</v>
-      </c>
-      <c r="C20" s="1">
-        <v>44295</v>
-      </c>
-      <c r="D20">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -993,7 +1081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
@@ -1006,25 +1094,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1047,7 +1135,7 @@
         <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1070,7 +1158,7 @@
         <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1093,7 +1181,7 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1116,7 +1204,7 @@
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added object id's to database excel download
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="57">
   <si>
     <t>User</t>
   </si>
@@ -94,6 +94,9 @@
     <t>start of 2022</t>
   </si>
   <si>
+    <t>SapID</t>
+  </si>
+  <si>
     <t>Tree</t>
   </si>
   <si>
@@ -106,6 +109,42 @@
     <t>Harvest Temp</t>
   </si>
   <si>
+    <t>"60776b61ccab402de07f4c81"</t>
+  </si>
+  <si>
+    <t>"60776e12ccab402de07f4c82"</t>
+  </si>
+  <si>
+    <t>"607787dc0eadad1a7868fe6c"</t>
+  </si>
+  <si>
+    <t>"607789ac06902a1e3881b27a"</t>
+  </si>
+  <si>
+    <t>"60778a8bd5577745f4085a06"</t>
+  </si>
+  <si>
+    <t>"60778b14e0edf5397cb584f6"</t>
+  </si>
+  <si>
+    <t>"60778bec5678c12dfc43ae5c"</t>
+  </si>
+  <si>
+    <t>"60778caa99ca002c28453020"</t>
+  </si>
+  <si>
+    <t>"60778d3663098e3e98890744"</t>
+  </si>
+  <si>
+    <t>"60778d889f9f3a3c6447bc04"</t>
+  </si>
+  <si>
+    <t>"6077974db6508a1cd0e0f073"</t>
+  </si>
+  <si>
+    <t>Syrup ID</t>
+  </si>
+  <si>
     <t>Syrup produced</t>
   </si>
   <si>
@@ -127,13 +166,25 @@
     <t>Fuel Type</t>
   </si>
   <si>
+    <t>"605e40cd60e99e32004bb4dc"</t>
+  </si>
+  <si>
     <t>propane</t>
   </si>
   <si>
+    <t>"6064f27d5320e055844a8c05"</t>
+  </si>
+  <si>
     <t>Propane</t>
   </si>
   <si>
+    <t>"60679b88c4170d31d476a7bb"</t>
+  </si>
+  <si>
     <t>Wood</t>
+  </si>
+  <si>
+    <t>"6070b6aa7d0400083c267385"</t>
   </si>
 </sst>
 </file>
@@ -901,13 +952,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="4" width="10" customWidth="1"/>
+    <col min="1" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -920,158 +971,194 @@
       <c r="D1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>12</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>44300</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>32</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>44302</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>44301</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>44308</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>8</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>44302</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>56</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>44310</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>4</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>44306</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>43</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>44291</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>67</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>44308</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>67</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>44314</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>67</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>44671</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>54</v>
       </c>
     </row>
@@ -1083,128 +1170,158 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="1" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
         <v>44281</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>36</v>
       </c>
-      <c r="G2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3">
         <v>100</v>
       </c>
-      <c r="B3">
+      <c r="D3">
         <v>1000</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44286</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
+        <v>44286</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
         <v>50</v>
       </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="I3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="D4">
         <v>15</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F4" s="1">
         <v>44288</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>22</v>
       </c>
-      <c r="G4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="F5" s="1">
         <v>44295</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
-        <v>38</v>
+      <c r="I5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Admin can now delete any data and its 'child' data by ID
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
   <si>
     <t>User</t>
   </si>
@@ -73,27 +73,9 @@
     <t>first season noteess</t>
   </si>
   <si>
-    <t>tree34</t>
-  </si>
-  <si>
-    <t>start of 2023</t>
-  </si>
-  <si>
-    <t>very long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notesvery long notes</t>
-  </si>
-  <si>
     <t>Season</t>
   </si>
   <si>
-    <t>starting a new tree</t>
-  </si>
-  <si>
-    <t>end of season 2021</t>
-  </si>
-  <si>
-    <t>start of 2022</t>
-  </si>
-  <si>
     <t>SapID</t>
   </si>
   <si>
@@ -109,37 +91,31 @@
     <t>Harvest Temp</t>
   </si>
   <si>
-    <t>"60776b61ccab402de07f4c81"</t>
-  </si>
-  <si>
-    <t>"60776e12ccab402de07f4c82"</t>
-  </si>
-  <si>
-    <t>"607787dc0eadad1a7868fe6c"</t>
-  </si>
-  <si>
-    <t>"607789ac06902a1e3881b27a"</t>
-  </si>
-  <si>
-    <t>"60778a8bd5577745f4085a06"</t>
-  </si>
-  <si>
-    <t>"60778b14e0edf5397cb584f6"</t>
-  </si>
-  <si>
-    <t>"60778bec5678c12dfc43ae5c"</t>
-  </si>
-  <si>
-    <t>"60778caa99ca002c28453020"</t>
-  </si>
-  <si>
-    <t>"60778d3663098e3e98890744"</t>
-  </si>
-  <si>
-    <t>"60778d889f9f3a3c6447bc04"</t>
-  </si>
-  <si>
-    <t>"6077974db6508a1cd0e0f073"</t>
+    <t>60776e12ccab402de07f4c82</t>
+  </si>
+  <si>
+    <t>607787dc0eadad1a7868fe6c</t>
+  </si>
+  <si>
+    <t>607789ac06902a1e3881b27a</t>
+  </si>
+  <si>
+    <t>60778a8bd5577745f4085a06</t>
+  </si>
+  <si>
+    <t>60778b14e0edf5397cb584f6</t>
+  </si>
+  <si>
+    <t>60778bec5678c12dfc43ae5c</t>
+  </si>
+  <si>
+    <t>60778caa99ca002c28453020</t>
+  </si>
+  <si>
+    <t>60778d3663098e3e98890744</t>
+  </si>
+  <si>
+    <t>60778d889f9f3a3c6447bc04</t>
   </si>
   <si>
     <t>Syrup ID</t>
@@ -166,25 +142,16 @@
     <t>Fuel Type</t>
   </si>
   <si>
-    <t>"605e40cd60e99e32004bb4dc"</t>
-  </si>
-  <si>
-    <t>propane</t>
-  </si>
-  <si>
-    <t>"6064f27d5320e055844a8c05"</t>
+    <t>60679b88c4170d31d476a7bb</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>6070b6aa7d0400083c267385</t>
   </si>
   <si>
     <t>Propane</t>
-  </si>
-  <si>
-    <t>"60679b88c4170d31d476a7bb"</t>
-  </si>
-  <si>
-    <t>Wood</t>
-  </si>
-  <si>
-    <t>"6070b6aa7d0400083c267385"</t>
   </si>
 </sst>
 </file>
@@ -562,7 +529,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="10" customWidth="1"/>
@@ -711,41 +678,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1">
-        <v>45000</v>
-      </c>
-      <c r="F5" s="1">
-        <v>44671</v>
-      </c>
-      <c r="G5" s="1">
-        <v>44671</v>
-      </c>
-      <c r="H5">
-        <v>39.399</v>
-      </c>
-      <c r="I5">
-        <v>-74.5146</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -754,7 +686,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="4" width="10" customWidth="1"/>
@@ -770,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -863,84 +795,6 @@
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>2021</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44301</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>2022</v>
-      </c>
-      <c r="D6" s="1">
-        <v>44664</v>
-      </c>
-      <c r="E6" s="1">
-        <v>44671</v>
-      </c>
-      <c r="F6" s="1">
-        <v>44671</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>2023</v>
-      </c>
-      <c r="D7" s="1">
-        <v>45000</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -952,7 +806,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="10" customWidth="1"/>
@@ -960,33 +814,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1">
-        <v>44300</v>
+        <v>44302</v>
       </c>
       <c r="E2">
         <v>49</v>
@@ -994,16 +848,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
-        <v>44302</v>
+        <v>44301</v>
       </c>
       <c r="E3">
         <v>49</v>
@@ -1011,16 +865,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>44301</v>
+        <v>44308</v>
       </c>
       <c r="E4">
         <v>49</v>
@@ -1028,16 +882,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
-        <v>44308</v>
+        <v>44302</v>
       </c>
       <c r="E5">
         <v>49</v>
@@ -1045,16 +899,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D6" s="1">
-        <v>44302</v>
+        <v>44310</v>
       </c>
       <c r="E6">
         <v>49</v>
@@ -1062,16 +916,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
-        <v>44310</v>
+        <v>44306</v>
       </c>
       <c r="E7">
         <v>49</v>
@@ -1079,16 +933,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1">
-        <v>44306</v>
+        <v>44291</v>
       </c>
       <c r="E8">
         <v>49</v>
@@ -1096,16 +950,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="D9" s="1">
-        <v>44291</v>
+        <v>44308</v>
       </c>
       <c r="E9">
         <v>49</v>
@@ -1113,7 +967,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -1122,44 +976,10 @@
         <v>67</v>
       </c>
       <c r="D10" s="1">
-        <v>44308</v>
+        <v>44314</v>
       </c>
       <c r="E10">
         <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>67</v>
-      </c>
-      <c r="D11" s="1">
-        <v>44314</v>
-      </c>
-      <c r="E11">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <v>67</v>
-      </c>
-      <c r="D12" s="1">
-        <v>44671</v>
-      </c>
-      <c r="E12">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1170,7 +990,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="10" customWidth="1"/>
@@ -1181,147 +1001,89 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
       <c r="C2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1">
-        <v>44281</v>
+        <v>44288</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
       <c r="H2">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
       <c r="C3">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1">
-        <v>44286</v>
+        <v>44295</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44288</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1">
-        <v>44295</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added bug fixes, added mongoDB backup
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>User</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>Harvest Temp</t>
-  </si>
-  <si>
-    <t>60776e12ccab402de07f4c82</t>
   </si>
   <si>
     <t>607787dc0eadad1a7868fe6c</t>
@@ -868,7 +865,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="10" customWidth="1"/>
@@ -896,13 +893,13 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
-        <v>44302</v>
+        <v>44301</v>
       </c>
       <c r="E2">
         <v>49</v>
@@ -916,10 +913,10 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
-        <v>44301</v>
+        <v>44308</v>
       </c>
       <c r="E3">
         <v>49</v>
@@ -933,10 +930,10 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1">
-        <v>44308</v>
+        <v>44302</v>
       </c>
       <c r="E4">
         <v>49</v>
@@ -950,10 +947,10 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D5" s="1">
-        <v>44302</v>
+        <v>44310</v>
       </c>
       <c r="E5">
         <v>49</v>
@@ -967,10 +964,10 @@
         <v>17</v>
       </c>
       <c r="C6">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1">
-        <v>44310</v>
+        <v>44306</v>
       </c>
       <c r="E6">
         <v>49</v>
@@ -984,10 +981,10 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1">
-        <v>44306</v>
+        <v>44291</v>
       </c>
       <c r="E7">
         <v>49</v>
@@ -1001,10 +998,10 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1">
-        <v>44291</v>
+        <v>44308</v>
       </c>
       <c r="E8">
         <v>49</v>
@@ -1021,7 +1018,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="1">
-        <v>44308</v>
+        <v>44314</v>
       </c>
       <c r="E9">
         <v>49</v>
@@ -1035,13 +1032,13 @@
         <v>17</v>
       </c>
       <c r="C10">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1">
-        <v>44314</v>
+        <v>44306</v>
       </c>
       <c r="E10">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1052,10 +1049,10 @@
         <v>17</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1">
-        <v>44306</v>
+        <v>44308</v>
       </c>
       <c r="E11">
         <v>47</v>
@@ -1069,10 +1066,10 @@
         <v>17</v>
       </c>
       <c r="C12">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D12" s="1">
-        <v>44308</v>
+        <v>44310</v>
       </c>
       <c r="E12">
         <v>47</v>
@@ -1086,29 +1083,12 @@
         <v>17</v>
       </c>
       <c r="C13">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1">
-        <v>44310</v>
+        <v>44313</v>
       </c>
       <c r="E13">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>20</v>
-      </c>
-      <c r="D14" s="1">
-        <v>44313</v>
-      </c>
-      <c r="E14">
         <v>62</v>
       </c>
     </row>
@@ -1131,48 +1111,48 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>46</v>
-      </c>
-      <c r="I1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>50</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
       </c>
       <c r="F2" s="1">
         <v>44305</v>
@@ -1184,24 +1164,24 @@
         <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>56</v>
       </c>
       <c r="F3" s="1">
         <v>44311</v>
@@ -1213,7 +1193,7 @@
         <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated manuel's profile pic
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="58">
   <si>
     <t>User</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>End of season 2021 wat a shame</t>
+  </si>
+  <si>
+    <t>edfasd</t>
   </si>
   <si>
     <t>Season</t>
@@ -562,7 +565,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="10" customWidth="1"/>
@@ -711,6 +714,41 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44300</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>39.3989</v>
+      </c>
+      <c r="I5">
+        <v>-74.5145</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -719,7 +757,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="4" width="10" customWidth="1"/>
@@ -735,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -825,7 +863,7 @@
         <v>44314</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
@@ -854,6 +892,32 @@
         <v>18</v>
       </c>
       <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>2021</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44300</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -873,24 +937,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -907,7 +971,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -924,7 +988,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -941,7 +1005,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -958,7 +1022,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -975,7 +1039,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -992,7 +1056,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1009,7 +1073,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -1026,7 +1090,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -1043,7 +1107,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -1060,7 +1124,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -1077,7 +1141,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
@@ -1111,48 +1175,48 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1">
         <v>44305</v>
@@ -1164,24 +1228,24 @@
         <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1">
         <v>44311</v>
@@ -1193,7 +1257,7 @@
         <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixes, COL changes
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="59">
   <si>
     <t>User</t>
   </si>
@@ -79,6 +79,12 @@
     <t>edfasd</t>
   </si>
   <si>
+    <t>testingtree</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
     <t>Season</t>
   </si>
   <si>
@@ -128,9 +134,6 @@
   </si>
   <si>
     <t>607e0e2b122a9d2f1092b966</t>
-  </si>
-  <si>
-    <t>607e0e31122a9d2f1092b967</t>
   </si>
   <si>
     <t>6082f0fdd406c93b6011e755</t>
@@ -565,7 +568,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="10" customWidth="1"/>
@@ -749,6 +752,35 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>111</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44318</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -757,7 +789,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="4" width="10" customWidth="1"/>
@@ -773,7 +805,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -863,7 +895,7 @@
         <v>44314</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
@@ -918,6 +950,32 @@
         <v>16</v>
       </c>
       <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>2021</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44318</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -929,7 +987,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="10" customWidth="1"/>
@@ -937,24 +995,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -971,7 +1029,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -988,7 +1046,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -1005,7 +1063,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1022,7 +1080,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -1039,7 +1097,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -1056,7 +1114,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1073,7 +1131,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -1090,7 +1148,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -1107,7 +1165,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -1124,35 +1182,18 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1">
-        <v>44310</v>
+        <v>44313</v>
       </c>
       <c r="E12">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1">
-        <v>44313</v>
-      </c>
-      <c r="E13">
         <v>62</v>
       </c>
     </row>
@@ -1175,48 +1216,48 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F2" s="1">
         <v>44305</v>
@@ -1228,24 +1269,24 @@
         <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F3" s="1">
         <v>44311</v>
@@ -1257,7 +1298,7 @@
         <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>